<commit_message>
barotrauma implementation for web app
</commit_message>
<xml_diff>
--- a/Data/Barotrauma_Values_Pflugrath2021.xlsx
+++ b/Data/Barotrauma_Values_Pflugrath2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kleinschmidtgroup-my.sharepoint.com/personal/andrew_yoder_kleinschmidtgroup_com/Documents/Software/stryke/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{D505972F-177E-419D-9AFD-5E64DD4C46EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08057AA9-1C03-403C-BE62-255B392A1B55}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{D505972F-177E-419D-9AFD-5E64DD4C46EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425AA7F2-88AF-4BCF-8339-9B665F2687F5}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="2250" windowWidth="24255" windowHeight="14295" activeTab="1" xr2:uid="{45FDDFD1-D85F-4AC2-9A31-7F021E5D3863}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{45FDDFD1-D85F-4AC2-9A31-7F021E5D3863}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortal Injury" sheetId="2" r:id="rId1"/>
@@ -266,14 +266,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,6 +293,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,274 +619,274 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>-5.3010000000000002</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>4.8250000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>-5.72</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2.68</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>-3.3079999999999998</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>6.1950000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>-5.7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>1.99</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>-5.56</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>3.85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>-6.5060000000000002</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>4.6689999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>-3.9369999999999998</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>5.7229999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>-8.9260000000000002</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>3.9940000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>-7.33</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>-5.1180000000000003</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>2.927</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>-3.91</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>1.39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>-3.9260000000000002</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <v>1.9570000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>-4.9569999999999999</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <v>2.8380000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6">
         <v>0</v>
       </c>
     </row>
@@ -892,247 +899,245 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63422E6F-A233-49BB-A001-B60AD80DCEEE}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>-4.431</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>2.617</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>-8.5730000000000004</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2.9790000000000001</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>-8.8019999999999996</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>5.0970000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>-7.22</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>1.9770000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>-7.7</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>3.8780000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>-7.71</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>3.82</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>-4.657</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>3.41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>-6.0190000000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>1.825</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>-6.5919999999999996</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>1.488</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>-5.4379999999999997</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>1.1259999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>